<commit_message>
removing previous year materials
</commit_message>
<xml_diff>
--- a/SCHEDULE.xlsx
+++ b/SCHEDULE.xlsx
@@ -1,16 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavodeloscampos/GitHub/STT465/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>Week 1</t>
   </si>
@@ -72,12 +80,6 @@
     <t>Week 15</t>
   </si>
   <si>
-    <t>No class</t>
-  </si>
-  <si>
-    <t>Final project presentations</t>
-  </si>
-  <si>
     <t>HW1 due</t>
   </si>
   <si>
@@ -99,9 +101,6 @@
     <t>Midterm</t>
   </si>
   <si>
-    <t xml:space="preserve"> Proposal due</t>
-  </si>
-  <si>
     <t>1st class</t>
   </si>
   <si>
@@ -138,18 +137,12 @@
     <t>Ch. 6 (Gibbs Sampler)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Tentative Schedule STT465, Fall, 2015.</t>
-  </si>
-  <si>
     <t>Review of Linear Algebra</t>
   </si>
   <si>
     <t>OLS Regression</t>
   </si>
   <si>
-    <t>ML &amp; MVN Dsitribution</t>
-  </si>
-  <si>
     <t>Ch. 9, Bayesian Multiple Linear Regression</t>
   </si>
   <si>
@@ -165,31 +158,34 @@
     <t>Gibbs Sampler with Fixed and Random EFFECS</t>
   </si>
   <si>
-    <t>Gibbs Sampler with scalar updates</t>
-  </si>
-  <si>
     <t>Dealing with missing values</t>
   </si>
   <si>
-    <t>Censored &amp; Binary outcomes</t>
-  </si>
-  <si>
-    <t>Final Project Due</t>
-  </si>
-  <si>
-    <t>Variable Selection in Linear Models</t>
-  </si>
-  <si>
     <t>Metropolis Hastings</t>
   </si>
   <si>
-    <t>Almeida, Schneider, Yau; Yanfeng, Liu, Park, Rykse</t>
-  </si>
-  <si>
-    <t>No Class</t>
-  </si>
-  <si>
-    <t>Catton, Hu, Lawrence, Suing, Hank, Gil, Vanamberg (12:45pm - 2:45pm in A120 Wells Hall)</t>
+    <t>No class, Labor Day</t>
+  </si>
+  <si>
+    <t>Final Eam Week</t>
+  </si>
+  <si>
+    <t>Maximum Likelihood Under Normality</t>
+  </si>
+  <si>
+    <t>Regression with Censored Outcomes</t>
+  </si>
+  <si>
+    <t>Regression with Binary Outcomes</t>
+  </si>
+  <si>
+    <t>H5 Posted</t>
+  </si>
+  <si>
+    <t>H5 Due</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tentative Schedule STT465, Fall, 2016.</t>
   </si>
 </sst>
 </file>
@@ -588,6 +584,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -602,9 +601,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="102">
@@ -713,6 +709,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1043,11 +1044,11 @@
   </sheetPr>
   <dimension ref="B2:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="4" max="4" width="10.1640625" style="1" customWidth="1"/>
@@ -1056,32 +1057,32 @@
     <col min="7" max="7" width="3.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="23">
+    <row r="2" spans="2:6" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="21" thickBot="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="22" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
     </row>
-    <row r="4" spans="2:6" ht="26" customHeight="1" thickBot="1">
+    <row r="4" spans="2:6" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="E4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="21" customHeight="1">
+    </row>
+    <row r="5" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
         <v>0</v>
       </c>
@@ -1089,30 +1090,30 @@
         <v>8</v>
       </c>
       <c r="D5" s="12">
-        <v>42249</v>
+        <v>42613</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="21" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="14"/>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3">
         <f>+D5+5</f>
-        <v>42254</v>
+        <v>42618</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="21" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
@@ -1121,58 +1122,58 @@
       </c>
       <c r="D7" s="3">
         <f>+D6+2</f>
-        <v>42256</v>
+        <v>42620</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="21" customHeight="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="17"/>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="5">
         <f>+D7+5</f>
-        <v>42261</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>31</v>
+        <v>42625</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>28</v>
       </c>
       <c r="F8" s="18"/>
     </row>
-    <row r="9" spans="2:6" ht="21" customHeight="1">
+    <row r="9" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17"/>
       <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="5">
         <f>+D8+2</f>
-        <v>42263</v>
-      </c>
-      <c r="E9" s="38"/>
+        <v>42627</v>
+      </c>
+      <c r="E9" s="39"/>
       <c r="F9" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="21" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="14"/>
       <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3">
         <f>+D9+5</f>
-        <v>42268</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>32</v>
+        <v>42632</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>29</v>
       </c>
       <c r="F10" s="16"/>
     </row>
-    <row r="11" spans="2:6" ht="21" customHeight="1">
+    <row r="11" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
         <v>2</v>
       </c>
@@ -1181,28 +1182,28 @@
       </c>
       <c r="D11" s="3">
         <f>+D10+2</f>
-        <v>42270</v>
-      </c>
-      <c r="E11" s="38"/>
+        <v>42634</v>
+      </c>
+      <c r="E11" s="39"/>
       <c r="F11" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="21" customHeight="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="17"/>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="5">
         <f>+D11+5</f>
-        <v>42275</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>33</v>
+        <v>42639</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>30</v>
       </c>
       <c r="F12" s="18"/>
     </row>
-    <row r="13" spans="2:6" ht="21" customHeight="1">
+    <row r="13" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>3</v>
       </c>
@@ -1211,28 +1212,28 @@
       </c>
       <c r="D13" s="5">
         <f>+D12+2</f>
-        <v>42277</v>
-      </c>
-      <c r="E13" s="38"/>
+        <v>42641</v>
+      </c>
+      <c r="E13" s="39"/>
       <c r="F13" s="18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="21" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="14"/>
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3">
         <f>+D13+5</f>
-        <v>42282</v>
-      </c>
-      <c r="E14" s="39" t="s">
-        <v>38</v>
+        <v>42646</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>35</v>
       </c>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="2:6" ht="21" customHeight="1">
+    <row r="15" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="14" t="s">
         <v>4</v>
       </c>
@@ -1241,28 +1242,28 @@
       </c>
       <c r="D15" s="3">
         <f>+D14+2</f>
-        <v>42284</v>
-      </c>
-      <c r="E15" s="38"/>
+        <v>42648</v>
+      </c>
+      <c r="E15" s="39"/>
       <c r="F15" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="21" customHeight="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="17"/>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="5">
         <f>+D15+5</f>
-        <v>42289</v>
+        <v>42653</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F16" s="18"/>
     </row>
-    <row r="17" spans="2:16" ht="21" customHeight="1">
+    <row r="17" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="17" t="s">
         <v>5</v>
       </c>
@@ -1271,30 +1272,30 @@
       </c>
       <c r="D17" s="5">
         <f>+D16+2</f>
-        <v>42291</v>
+        <v>42655</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" ht="26" customHeight="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="14"/>
       <c r="C18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3">
         <f>+D17+5</f>
-        <v>42296</v>
+        <v>42660</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F18" s="16"/>
     </row>
-    <row r="19" spans="2:16" ht="21" customHeight="1">
+    <row r="19" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="14" t="s">
         <v>6</v>
       </c>
@@ -1303,28 +1304,28 @@
       </c>
       <c r="D19" s="3">
         <f>+D18+2</f>
-        <v>42298</v>
+        <v>42662</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" spans="2:16" ht="21" customHeight="1">
+    <row r="20" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="17"/>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="5">
         <f>+D19+5</f>
-        <v>42303</v>
+        <v>42667</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F20" s="18"/>
     </row>
-    <row r="21" spans="2:16" ht="21" customHeight="1">
+    <row r="21" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="17" t="s">
         <v>7</v>
       </c>
@@ -1333,32 +1334,32 @@
       </c>
       <c r="D21" s="5">
         <f>+D20+2</f>
-        <v>42305</v>
+        <v>42669</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" ht="21" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="14"/>
       <c r="C22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3">
         <f>+D21+5</f>
-        <v>42310</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>47</v>
+        <v>42674</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>42</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" ht="21" customHeight="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="14" t="s">
         <v>10</v>
       </c>
@@ -1367,38 +1368,36 @@
       </c>
       <c r="D23" s="3">
         <f>+D22+2</f>
-        <v>42312</v>
-      </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
+        <v>42676</v>
+      </c>
+      <c r="E23" s="39"/>
+      <c r="F23" s="16"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
       <c r="P23" s="35"/>
     </row>
-    <row r="24" spans="2:16" ht="21" customHeight="1">
+    <row r="24" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="17"/>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="5">
         <f>+D23+5</f>
-        <v>42317</v>
-      </c>
-      <c r="E24" s="37" t="s">
-        <v>48</v>
+        <v>42681</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>43</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" ht="21" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="17" t="s">
         <v>11</v>
       </c>
@@ -1407,26 +1406,28 @@
       </c>
       <c r="D25" s="5">
         <f>+D24+2</f>
-        <v>42319</v>
-      </c>
-      <c r="E25" s="38"/>
+        <v>42683</v>
+      </c>
+      <c r="E25" s="39"/>
       <c r="F25" s="18"/>
     </row>
-    <row r="26" spans="2:16" ht="21" customHeight="1">
+    <row r="26" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="14"/>
       <c r="C26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3">
         <f>+D25+5</f>
-        <v>42324</v>
-      </c>
-      <c r="E26" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="F26" s="16"/>
-    </row>
-    <row r="27" spans="2:16" ht="21" customHeight="1">
+        <v>42688</v>
+      </c>
+      <c r="E26" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="14" t="s">
         <v>12</v>
       </c>
@@ -1435,26 +1436,26 @@
       </c>
       <c r="D27" s="3">
         <f>+D26+2</f>
-        <v>42326</v>
-      </c>
-      <c r="E27" s="38"/>
+        <v>42690</v>
+      </c>
+      <c r="E27" s="39"/>
       <c r="F27" s="16"/>
     </row>
-    <row r="28" spans="2:16" ht="21" customHeight="1">
+    <row r="28" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="17"/>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="5">
         <f>+D27+5</f>
-        <v>42331</v>
-      </c>
-      <c r="E28" s="37" t="s">
-        <v>50</v>
+        <v>42695</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>49</v>
       </c>
       <c r="F28" s="18"/>
     </row>
-    <row r="29" spans="2:16" ht="21" customHeight="1">
+    <row r="29" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="17" t="s">
         <v>13</v>
       </c>
@@ -1463,26 +1464,28 @@
       </c>
       <c r="D29" s="5">
         <f>+D28+2</f>
-        <v>42333</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" spans="2:16" ht="21" customHeight="1">
+        <v>42697</v>
+      </c>
+      <c r="E29" s="39"/>
+      <c r="F29" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="14"/>
       <c r="C30" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3">
         <f>+D29+5</f>
-        <v>42338</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>52</v>
+        <v>42702</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>44</v>
       </c>
       <c r="F30" s="16"/>
     </row>
-    <row r="31" spans="2:16" ht="21" customHeight="1">
+    <row r="31" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="14" t="s">
         <v>14</v>
       </c>
@@ -1491,30 +1494,26 @@
       </c>
       <c r="D31" s="3">
         <f>+D30+2</f>
-        <v>42340</v>
-      </c>
-      <c r="E31" s="38"/>
+        <v>42704</v>
+      </c>
+      <c r="E31" s="39"/>
       <c r="F31" s="16"/>
       <c r="H31" s="32"/>
     </row>
-    <row r="32" spans="2:16" ht="21" customHeight="1">
+    <row r="32" spans="2:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="17"/>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="5">
         <f>+D31+5</f>
-        <v>42345</v>
-      </c>
-      <c r="E32" s="34" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="31" t="s">
-        <v>51</v>
-      </c>
+        <v>42709</v>
+      </c>
+      <c r="E32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="H32" s="32"/>
     </row>
-    <row r="33" spans="2:6" ht="21" customHeight="1">
+    <row r="33" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="17" t="s">
         <v>15</v>
       </c>
@@ -1523,30 +1522,26 @@
       </c>
       <c r="D33" s="5">
         <f>+D32+2</f>
-        <v>42347</v>
-      </c>
-      <c r="E33" s="34" t="s">
-        <v>54</v>
-      </c>
+        <v>42711</v>
+      </c>
+      <c r="E33" s="34"/>
       <c r="F33" s="31"/>
     </row>
-    <row r="34" spans="2:6" ht="21" customHeight="1">
+    <row r="34" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="14"/>
       <c r="C34" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="3">
         <f>+D33+5</f>
-        <v>42352</v>
-      </c>
-      <c r="E34" s="33" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="40" customHeight="1">
+        <v>42716</v>
+      </c>
+      <c r="E34" s="33"/>
+      <c r="F34" s="41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="19" t="s">
         <v>16</v>
       </c>
@@ -1555,34 +1550,27 @@
       </c>
       <c r="D35" s="21">
         <f>+D34+2</f>
-        <v>42354</v>
-      </c>
-      <c r="E35" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="41"/>
+        <v>42718</v>
+      </c>
+      <c r="E35" s="36"/>
+      <c r="F35" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="I23:O23"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="E30:E31"/>
     <mergeCell ref="F34:F35"/>
     <mergeCell ref="E24:E25"/>
     <mergeCell ref="E26:E27"/>
+    <mergeCell ref="I23:O23"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="40" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>